<commit_message>
Corrected negative values in Cat_tot
</commit_message>
<xml_diff>
--- a/Multi-taxa_data/PLITs/extraction/PLIT_G1.xlsx
+++ b/Multi-taxa_data/PLITs/extraction/PLIT_G1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\COMUNE\STUDIO.LAVORO\IMBRSea\Thesis\StatAnalysis\Multi-taxa_data\PLITs\extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97570E84-F2BE-497C-9C4B-C65F792EEA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771F0165-936E-40A0-867B-F1E44E72EDBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1892,7 +1892,7 @@
   <dimension ref="A1:U235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="C5" sqref="C5:C150"/>
@@ -5253,10 +5253,10 @@
   <dimension ref="A1:U235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E134" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E146" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5:C151"/>
+      <selection pane="bottomRight" activeCell="A153" sqref="A153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7091,7 +7091,7 @@
       </c>
       <c r="C97" s="6">
         <f t="shared" si="1"/>
-        <v>147</v>
+        <v>47</v>
       </c>
       <c r="D97" s="6"/>
       <c r="K97" s="1" t="s">
@@ -7100,14 +7100,14 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="6">
-        <v>1797</v>
+        <v>1697</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C98" s="6">
         <f t="shared" si="1"/>
-        <v>-89</v>
+        <v>11</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>36</v>
@@ -8057,15 +8057,14 @@
       <c r="A152" s="6">
         <v>2531</v>
       </c>
-      <c r="B152" s="6" t="s">
-        <v>123</v>
-      </c>
       <c r="C152" s="6"/>
       <c r="D152" s="6"/>
       <c r="K152" s="6"/>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A153" s="6"/>
+      <c r="A153" s="6" t="s">
+        <v>123</v>
+      </c>
       <c r="B153" s="6"/>
       <c r="C153" s="6"/>
       <c r="D153" s="6"/>
@@ -8657,7 +8656,7 @@
       <pane xSplit="4" ySplit="4" topLeftCell="E148" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5:C166"/>
+      <selection pane="bottomRight" activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11737,15 +11736,14 @@
       <c r="A167" s="6">
         <v>2515</v>
       </c>
-      <c r="B167" s="6" t="s">
-        <v>123</v>
-      </c>
       <c r="C167" s="6"/>
       <c r="D167" s="6"/>
       <c r="K167" s="6"/>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A168" s="6"/>
+      <c r="A168" s="6" t="s">
+        <v>123</v>
+      </c>
       <c r="B168" s="6"/>
       <c r="C168" s="6"/>
       <c r="D168" s="6"/>
@@ -12231,7 +12229,7 @@
       <pane xSplit="4" ySplit="4" topLeftCell="E91" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B108" sqref="B108"/>
+      <selection pane="bottomRight" activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -14281,15 +14279,14 @@
       <c r="A108" s="6">
         <v>1100</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="C108" s="6"/>
       <c r="D108" s="6"/>
       <c r="K108" s="6"/>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A109" s="6"/>
+      <c r="A109" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
       <c r="D109" s="6"/>
@@ -15191,10 +15188,10 @@
   <dimension ref="A1:U234"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E130" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E136" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5:C148"/>
+      <selection pane="bottomRight" activeCell="A150" sqref="A150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -18943,9 +18940,6 @@
       <c r="A149" s="21">
         <v>2585</v>
       </c>
-      <c r="B149" s="22" t="s">
-        <v>123</v>
-      </c>
       <c r="C149" s="22"/>
       <c r="D149" s="22"/>
       <c r="E149" s="22"/>
@@ -18958,7 +18952,9 @@
       <c r="L149" s="22"/>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A150" s="6"/>
+      <c r="A150" s="22" t="s">
+        <v>123</v>
+      </c>
       <c r="B150" s="6"/>
       <c r="C150" s="6"/>
       <c r="D150" s="6"/>
@@ -19565,8 +19561,8 @@
   </sheetPr>
   <dimension ref="A1:U235"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="G119" sqref="F119:G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -20047,7 +20043,7 @@
       </c>
       <c r="C18" s="22">
         <f t="shared" si="0"/>
-        <v>-90</v>
+        <v>10</v>
       </c>
       <c r="D18" s="22" t="s">
         <v>21</v>
@@ -20065,14 +20061,14 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="21">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="22">
         <f t="shared" si="0"/>
-        <v>285</v>
+        <v>185</v>
       </c>
       <c r="D19" s="22" t="s">
         <v>36</v>
@@ -21272,7 +21268,7 @@
       </c>
       <c r="C69" s="22">
         <f t="shared" si="0"/>
-        <v>-64</v>
+        <v>36</v>
       </c>
       <c r="D69" s="22"/>
       <c r="E69" s="22"/>
@@ -21288,14 +21284,14 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="21">
-        <v>1232</v>
+        <v>1332</v>
       </c>
       <c r="B70" s="22" t="s">
         <v>390</v>
       </c>
       <c r="C70" s="22">
         <f t="shared" ref="C70:C127" si="1">A71-A70</f>
-        <v>177</v>
+        <v>77</v>
       </c>
       <c r="D70" s="22"/>
       <c r="E70" s="22"/>
@@ -22723,9 +22719,6 @@
     <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" s="21">
         <v>2700</v>
-      </c>
-      <c r="B128" s="22" t="s">
-        <v>123</v>
       </c>
       <c r="C128" s="22"/>
       <c r="D128" s="22"/>
@@ -22739,7 +22732,9 @@
       <c r="L128" s="22"/>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A129" s="6"/>
+      <c r="A129" s="22" t="s">
+        <v>123</v>
+      </c>
       <c r="B129" s="6"/>
       <c r="C129" s="6"/>
       <c r="D129" s="6"/>

</xml_diff>

<commit_message>
filling missing functional groups
</commit_message>
<xml_diff>
--- a/Multi-taxa_data/PLITs/extraction/PLIT_G1.xlsx
+++ b/Multi-taxa_data/PLITs/extraction/PLIT_G1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\COMUNE\STUDIO.LAVORO\IMBRSea\Thesis\StatAnalysis\Multi-taxa_data\PLITs\extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D4029C-874F-4C95-98DB-650548295308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C3A663-AA0C-40A6-874E-BF9C73490CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="D1" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'D1'!$A$4:$U$151</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'S1'!$A$4:$U$189</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'S2'!$A$4:$U$149</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'S3'!$A$4:$U$129</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -12374,11 +12376,11 @@
   </sheetPr>
   <dimension ref="A1:U235"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="I170" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="I6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A190" sqref="A190"/>
+      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -16086,14 +16088,14 @@
       <c r="D217" s="6"/>
       <c r="K217" s="6"/>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A218" s="6"/>
       <c r="B218" s="6"/>
       <c r="C218" s="6"/>
       <c r="D218" s="6"/>
       <c r="K218" s="6"/>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A219" s="6"/>
       <c r="B219" s="6"/>
       <c r="C219" s="6"/>
@@ -16101,113 +16103,114 @@
       <c r="K219" s="6"/>
       <c r="L219" s="6"/>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A220" s="6"/>
       <c r="B220" s="6"/>
       <c r="C220" s="6"/>
       <c r="D220" s="6"/>
       <c r="K220" s="6"/>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A221" s="6"/>
       <c r="B221" s="6"/>
       <c r="C221" s="6"/>
       <c r="D221" s="6"/>
       <c r="K221" s="6"/>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A222" s="6"/>
       <c r="B222" s="6"/>
       <c r="C222" s="6"/>
       <c r="D222" s="6"/>
       <c r="K222" s="6"/>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A223" s="6"/>
       <c r="B223" s="6"/>
       <c r="C223" s="6"/>
       <c r="D223" s="6"/>
       <c r="K223" s="6"/>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A224" s="6"/>
       <c r="B224" s="6"/>
       <c r="C224" s="6"/>
       <c r="D224" s="6"/>
       <c r="K224" s="6"/>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A225" s="6"/>
       <c r="B225" s="6"/>
       <c r="C225" s="6"/>
       <c r="D225" s="6"/>
       <c r="K225" s="6"/>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A226" s="6"/>
       <c r="B226" s="6"/>
       <c r="C226" s="6"/>
       <c r="D226" s="6"/>
       <c r="K226" s="6"/>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A227" s="6"/>
       <c r="B227" s="6"/>
       <c r="C227" s="6"/>
       <c r="D227" s="6"/>
       <c r="K227" s="6"/>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A228" s="6"/>
       <c r="B228" s="6"/>
       <c r="C228" s="6"/>
       <c r="D228" s="6"/>
       <c r="K228" s="6"/>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A229" s="6"/>
       <c r="B229" s="6"/>
       <c r="C229" s="6"/>
       <c r="D229" s="6"/>
       <c r="K229" s="6"/>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A230" s="6"/>
       <c r="B230" s="6"/>
       <c r="C230" s="6"/>
       <c r="D230" s="6"/>
       <c r="K230" s="6"/>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A231" s="6"/>
       <c r="B231" s="6"/>
       <c r="C231" s="6"/>
       <c r="D231" s="6"/>
       <c r="K231" s="6"/>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A232" s="6"/>
       <c r="B232" s="6"/>
       <c r="C232" s="6"/>
       <c r="D232" s="6"/>
       <c r="K232" s="6"/>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A233" s="6"/>
       <c r="B233" s="6"/>
       <c r="C233" s="6"/>
       <c r="D233" s="6"/>
       <c r="K233" s="6"/>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A234" s="6"/>
       <c r="C234" s="6"/>
       <c r="K234" s="6"/>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A235" s="6"/>
     </row>
   </sheetData>
+  <autoFilter ref="A4:U189" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -16219,8 +16222,8 @@
   </sheetPr>
   <dimension ref="A1:U234"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E59" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="E108" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="B75" sqref="B75"/>
@@ -16241,7 +16244,7 @@
     <col min="12" max="22" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -16259,7 +16262,7 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -16277,7 +16280,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -16296,7 +16299,7 @@
       <c r="L3" s="3"/>
       <c r="O3" s="6"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
@@ -16341,7 +16344,7 @@
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="21">
         <v>0</v>
       </c>
@@ -16373,7 +16376,7 @@
       <c r="T5" s="6"/>
       <c r="U5" s="6"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
         <v>1</v>
       </c>
@@ -16400,7 +16403,7 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -16427,7 +16430,7 @@
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="21">
         <v>16</v>
       </c>
@@ -16458,7 +16461,7 @@
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="21">
         <v>21</v>
       </c>
@@ -16489,7 +16492,7 @@
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="21">
         <v>23</v>
       </c>
@@ -16516,7 +16519,7 @@
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="21">
         <v>27</v>
       </c>
@@ -16543,7 +16546,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="21">
         <v>48</v>
       </c>
@@ -16570,7 +16573,7 @@
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="21">
         <v>52</v>
       </c>
@@ -16597,7 +16600,7 @@
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="21">
         <v>67</v>
       </c>
@@ -16624,7 +16627,7 @@
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="21">
         <v>86</v>
       </c>
@@ -16651,7 +16654,7 @@
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="21">
         <v>102</v>
       </c>
@@ -16676,7 +16679,7 @@
       </c>
       <c r="L16" s="22"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="21">
         <v>107</v>
       </c>
@@ -16699,7 +16702,7 @@
       </c>
       <c r="L17" s="22"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="21">
         <v>118</v>
       </c>
@@ -16724,7 +16727,7 @@
       </c>
       <c r="L18" s="25"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="21">
         <v>120</v>
       </c>
@@ -16749,7 +16752,7 @@
       </c>
       <c r="L19" s="22"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="21">
         <v>124</v>
       </c>
@@ -16774,7 +16777,7 @@
       </c>
       <c r="L20" s="22"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="21">
         <v>127</v>
       </c>
@@ -16799,7 +16802,7 @@
       </c>
       <c r="L21" s="22"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="21">
         <v>150</v>
       </c>
@@ -16824,7 +16827,7 @@
       </c>
       <c r="L22" s="22"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="21">
         <v>165</v>
       </c>
@@ -16849,7 +16852,7 @@
       </c>
       <c r="L23" s="22"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="21">
         <v>169</v>
       </c>
@@ -16874,7 +16877,7 @@
       </c>
       <c r="L24" s="22"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="21">
         <v>190</v>
       </c>
@@ -16899,7 +16902,7 @@
       </c>
       <c r="L25" s="22"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="21">
         <v>196</v>
       </c>
@@ -16924,7 +16927,7 @@
       </c>
       <c r="L26" s="22"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="21">
         <v>210</v>
       </c>
@@ -16947,7 +16950,7 @@
       </c>
       <c r="L27" s="22"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="21">
         <v>222</v>
       </c>
@@ -16972,7 +16975,7 @@
       </c>
       <c r="L28" s="22"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="21">
         <v>227</v>
       </c>
@@ -16997,7 +17000,7 @@
       </c>
       <c r="L29" s="22"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="21">
         <v>240</v>
       </c>
@@ -17022,7 +17025,7 @@
       </c>
       <c r="L30" s="22"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="21">
         <v>278</v>
       </c>
@@ -17047,7 +17050,7 @@
       </c>
       <c r="L31" s="22"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="21">
         <v>281</v>
       </c>
@@ -17072,7 +17075,7 @@
       </c>
       <c r="L32" s="22"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="21">
         <v>288</v>
       </c>
@@ -17097,7 +17100,7 @@
       </c>
       <c r="L33" s="22"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="21">
         <v>291</v>
       </c>
@@ -17122,7 +17125,7 @@
       </c>
       <c r="L34" s="22"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="21">
         <v>298</v>
       </c>
@@ -17147,7 +17150,7 @@
       </c>
       <c r="L35" s="22"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="21">
         <v>301</v>
       </c>
@@ -17172,7 +17175,7 @@
       </c>
       <c r="L36" s="22"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="21">
         <v>304</v>
       </c>
@@ -17197,7 +17200,7 @@
       </c>
       <c r="L37" s="22"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="21">
         <v>307</v>
       </c>
@@ -17222,7 +17225,7 @@
       </c>
       <c r="L38" s="22"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="21">
         <v>346</v>
       </c>
@@ -17249,7 +17252,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="21">
         <v>380</v>
       </c>
@@ -17276,7 +17279,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="21">
         <v>399</v>
       </c>
@@ -17303,7 +17306,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="21">
         <v>440</v>
       </c>
@@ -17330,7 +17333,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="21">
         <v>488</v>
       </c>
@@ -17357,7 +17360,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="21">
         <v>491</v>
       </c>
@@ -17382,7 +17385,7 @@
       </c>
       <c r="L44" s="22"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="21">
         <v>493</v>
       </c>
@@ -17407,7 +17410,7 @@
       </c>
       <c r="L45" s="22"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="21">
         <v>497</v>
       </c>
@@ -17432,7 +17435,7 @@
       </c>
       <c r="L46" s="22"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="21">
         <v>504</v>
       </c>
@@ -17459,7 +17462,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="21">
         <v>510</v>
       </c>
@@ -17486,7 +17489,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="21">
         <v>514</v>
       </c>
@@ -17511,7 +17514,7 @@
       </c>
       <c r="L49" s="22"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="21">
         <v>524</v>
       </c>
@@ -17536,7 +17539,7 @@
       </c>
       <c r="L50" s="22"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="21">
         <v>533</v>
       </c>
@@ -17561,7 +17564,7 @@
       </c>
       <c r="L51" s="22"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="21">
         <v>558</v>
       </c>
@@ -17586,7 +17589,7 @@
       </c>
       <c r="L52" s="22"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="21">
         <v>559</v>
       </c>
@@ -17611,7 +17614,7 @@
       </c>
       <c r="L53" s="22"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="21">
         <v>621</v>
       </c>
@@ -17636,7 +17639,7 @@
       </c>
       <c r="L54" s="22"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="21">
         <v>625</v>
       </c>
@@ -17661,7 +17664,7 @@
       </c>
       <c r="L55" s="33"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="21">
         <v>660</v>
       </c>
@@ -17686,7 +17689,7 @@
       </c>
       <c r="L56" s="22"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="21">
         <v>663</v>
       </c>
@@ -17711,7 +17714,7 @@
       </c>
       <c r="L57" s="22"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="21">
         <v>667</v>
       </c>
@@ -17736,7 +17739,7 @@
       </c>
       <c r="L58" s="22"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="21">
         <v>689</v>
       </c>
@@ -17761,7 +17764,7 @@
       </c>
       <c r="L59" s="22"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="21">
         <v>692</v>
       </c>
@@ -17786,7 +17789,7 @@
       </c>
       <c r="L60" s="22"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="21">
         <v>695</v>
       </c>
@@ -17811,7 +17814,7 @@
       </c>
       <c r="L61" s="22"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="21">
         <v>697</v>
       </c>
@@ -17836,7 +17839,7 @@
       </c>
       <c r="L62" s="22"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="21">
         <v>703</v>
       </c>
@@ -17861,7 +17864,7 @@
       </c>
       <c r="L63" s="22"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="21">
         <v>712</v>
       </c>
@@ -17886,7 +17889,7 @@
       </c>
       <c r="L64" s="25"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="21">
         <v>716</v>
       </c>
@@ -17911,7 +17914,7 @@
       </c>
       <c r="L65" s="22"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="21">
         <v>718</v>
       </c>
@@ -17936,7 +17939,7 @@
       </c>
       <c r="L66" s="22"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="21">
         <v>722</v>
       </c>
@@ -17961,7 +17964,7 @@
       </c>
       <c r="L67" s="22"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="21">
         <v>759</v>
       </c>
@@ -17986,7 +17989,7 @@
       </c>
       <c r="L68" s="22"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="21">
         <v>764</v>
       </c>
@@ -18011,7 +18014,7 @@
       </c>
       <c r="L69" s="22"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="21">
         <v>767</v>
       </c>
@@ -18034,7 +18037,7 @@
       </c>
       <c r="L70" s="22"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="21">
         <v>774</v>
       </c>
@@ -18059,7 +18062,7 @@
       </c>
       <c r="L71" s="22"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="21">
         <v>782</v>
       </c>
@@ -18084,7 +18087,7 @@
       </c>
       <c r="L72" s="22"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="21">
         <v>786</v>
       </c>
@@ -18109,7 +18112,7 @@
       </c>
       <c r="L73" s="22"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="21">
         <v>789</v>
       </c>
@@ -18134,7 +18137,7 @@
       </c>
       <c r="L74" s="22"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="21">
         <v>791</v>
       </c>
@@ -18159,7 +18162,7 @@
       </c>
       <c r="L75" s="22"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="21">
         <v>794</v>
       </c>
@@ -18184,7 +18187,7 @@
       </c>
       <c r="L76" s="22"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="21">
         <v>808</v>
       </c>
@@ -18209,7 +18212,7 @@
       </c>
       <c r="L77" s="22"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="21">
         <v>872</v>
       </c>
@@ -18234,7 +18237,7 @@
       </c>
       <c r="L78" s="22"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="21">
         <v>889</v>
       </c>
@@ -18259,7 +18262,7 @@
       </c>
       <c r="L79" s="22"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="21">
         <v>892</v>
       </c>
@@ -18284,7 +18287,7 @@
       </c>
       <c r="L80" s="22"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="21">
         <v>894</v>
       </c>
@@ -18307,7 +18310,7 @@
       </c>
       <c r="L81" s="22"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="21">
         <v>899</v>
       </c>
@@ -18332,7 +18335,7 @@
       </c>
       <c r="L82" s="22"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="21">
         <v>920</v>
       </c>
@@ -18355,7 +18358,7 @@
       </c>
       <c r="L83" s="22"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="21">
         <v>944</v>
       </c>
@@ -18380,7 +18383,7 @@
       </c>
       <c r="L84" s="22"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="21">
         <v>948</v>
       </c>
@@ -18405,7 +18408,7 @@
       </c>
       <c r="L85" s="22"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="21">
         <v>963</v>
       </c>
@@ -18430,7 +18433,7 @@
       </c>
       <c r="L86" s="22"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="21">
         <v>981</v>
       </c>
@@ -18455,7 +18458,7 @@
       </c>
       <c r="L87" s="22"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="21">
         <v>997</v>
       </c>
@@ -18480,7 +18483,7 @@
       </c>
       <c r="L88" s="22"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="21">
         <v>1027</v>
       </c>
@@ -18505,7 +18508,7 @@
       </c>
       <c r="L89" s="22"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="21">
         <v>1062</v>
       </c>
@@ -18530,7 +18533,7 @@
       </c>
       <c r="L90" s="22"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="21">
         <v>1090</v>
       </c>
@@ -18555,7 +18558,7 @@
       </c>
       <c r="L91" s="22"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="21">
         <v>1116</v>
       </c>
@@ -18580,7 +18583,7 @@
       </c>
       <c r="L92" s="22"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="21">
         <v>1158</v>
       </c>
@@ -18605,7 +18608,7 @@
       </c>
       <c r="L93" s="22"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="21">
         <v>1163</v>
       </c>
@@ -18630,7 +18633,7 @@
       </c>
       <c r="L94" s="22"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="21">
         <v>1177</v>
       </c>
@@ -18655,7 +18658,7 @@
       </c>
       <c r="L95" s="22"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="21">
         <v>1182</v>
       </c>
@@ -18680,7 +18683,7 @@
       </c>
       <c r="L96" s="22"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="21">
         <v>1184</v>
       </c>
@@ -18705,7 +18708,7 @@
       </c>
       <c r="L97" s="22"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="21">
         <v>1227</v>
       </c>
@@ -18730,7 +18733,7 @@
       </c>
       <c r="L98" s="22"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="21">
         <v>1247</v>
       </c>
@@ -18755,7 +18758,7 @@
       </c>
       <c r="L99" s="22"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="21">
         <v>1268</v>
       </c>
@@ -18780,7 +18783,7 @@
       </c>
       <c r="L100" s="22"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="21">
         <v>1277</v>
       </c>
@@ -18805,7 +18808,7 @@
       </c>
       <c r="L101" s="22"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="21">
         <v>1280</v>
       </c>
@@ -18830,7 +18833,7 @@
       </c>
       <c r="L102" s="22"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="21">
         <v>1299</v>
       </c>
@@ -18855,7 +18858,7 @@
       </c>
       <c r="L103" s="22"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="21">
         <v>1341</v>
       </c>
@@ -18880,7 +18883,7 @@
       </c>
       <c r="L104" s="22"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="21">
         <v>1343</v>
       </c>
@@ -18905,7 +18908,7 @@
       </c>
       <c r="L105" s="22"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="21">
         <v>1369</v>
       </c>
@@ -18930,7 +18933,7 @@
       </c>
       <c r="L106" s="22"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="21">
         <v>1372</v>
       </c>
@@ -18955,7 +18958,7 @@
       </c>
       <c r="L107" s="33"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="21">
         <v>1463</v>
       </c>
@@ -18980,7 +18983,7 @@
       </c>
       <c r="L108" s="22"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="21">
         <v>1467</v>
       </c>
@@ -19005,7 +19008,7 @@
       </c>
       <c r="L109" s="22"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" s="21">
         <v>1476</v>
       </c>
@@ -19030,7 +19033,7 @@
       </c>
       <c r="L110" s="22"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="21">
         <v>1485</v>
       </c>
@@ -19055,7 +19058,7 @@
       </c>
       <c r="L111" s="22"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="21">
         <v>1530</v>
       </c>
@@ -19080,7 +19083,7 @@
       </c>
       <c r="L112" s="22"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="21">
         <v>1567</v>
       </c>
@@ -19105,7 +19108,7 @@
       </c>
       <c r="L113" s="22"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="21">
         <v>1584</v>
       </c>
@@ -19130,7 +19133,7 @@
       </c>
       <c r="L114" s="22"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="21">
         <v>1590</v>
       </c>
@@ -19155,7 +19158,7 @@
       </c>
       <c r="L115" s="22"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="21">
         <v>1596</v>
       </c>
@@ -19180,7 +19183,7 @@
       </c>
       <c r="L116" s="22"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="21">
         <v>1601</v>
       </c>
@@ -19205,7 +19208,7 @@
       </c>
       <c r="L117" s="22"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="21">
         <v>1618</v>
       </c>
@@ -19230,7 +19233,7 @@
       </c>
       <c r="L118" s="22"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="21">
         <v>1643</v>
       </c>
@@ -19255,7 +19258,7 @@
       </c>
       <c r="L119" s="22"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="21">
         <v>1670</v>
       </c>
@@ -19280,7 +19283,7 @@
       </c>
       <c r="L120" s="22"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="21">
         <v>1690</v>
       </c>
@@ -19305,7 +19308,7 @@
       </c>
       <c r="L121" s="33"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="21">
         <v>2092</v>
       </c>
@@ -19330,7 +19333,7 @@
       </c>
       <c r="L122" s="22"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="21">
         <v>2095</v>
       </c>
@@ -19355,7 +19358,7 @@
       </c>
       <c r="L123" s="22"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="21">
         <v>2139</v>
       </c>
@@ -19380,7 +19383,7 @@
       </c>
       <c r="L124" s="22"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="21">
         <v>2149</v>
       </c>
@@ -19405,7 +19408,7 @@
       </c>
       <c r="L125" s="22"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" s="21">
         <v>2180</v>
       </c>
@@ -19430,7 +19433,7 @@
       </c>
       <c r="L126" s="22"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A127" s="21">
         <v>2192</v>
       </c>
@@ -19455,7 +19458,7 @@
       </c>
       <c r="L127" s="22"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A128" s="21">
         <v>2218</v>
       </c>
@@ -19480,7 +19483,7 @@
       </c>
       <c r="L128" s="22"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A129" s="21">
         <v>2221</v>
       </c>
@@ -19503,7 +19506,7 @@
       </c>
       <c r="L129" s="22"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" s="21">
         <v>2225</v>
       </c>
@@ -19528,7 +19531,7 @@
       </c>
       <c r="L130" s="22"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="21">
         <v>2241</v>
       </c>
@@ -19551,7 +19554,7 @@
       </c>
       <c r="L131" s="22"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="21">
         <v>2283</v>
       </c>
@@ -19576,7 +19579,7 @@
       </c>
       <c r="L132" s="22"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="21">
         <v>2308</v>
       </c>
@@ -19601,7 +19604,7 @@
       </c>
       <c r="L133" s="22"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="21">
         <v>2331</v>
       </c>
@@ -19626,7 +19629,7 @@
       </c>
       <c r="L134" s="22"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A135" s="21">
         <v>2333</v>
       </c>
@@ -19649,7 +19652,7 @@
       </c>
       <c r="L135" s="22"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A136" s="21">
         <v>2335</v>
       </c>
@@ -19674,7 +19677,7 @@
       </c>
       <c r="L136" s="22"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A137" s="21">
         <v>2346</v>
       </c>
@@ -19699,7 +19702,7 @@
       </c>
       <c r="L137" s="22"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A138" s="21">
         <v>2360</v>
       </c>
@@ -19724,7 +19727,7 @@
       </c>
       <c r="L138" s="22"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A139" s="21">
         <v>2377</v>
       </c>
@@ -19749,7 +19752,7 @@
       </c>
       <c r="L139" s="22"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" s="21">
         <v>2390</v>
       </c>
@@ -19774,7 +19777,7 @@
       </c>
       <c r="L140" s="22"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A141" s="21">
         <v>2404</v>
       </c>
@@ -19797,7 +19800,7 @@
       </c>
       <c r="L141" s="22"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="21">
         <v>2408</v>
       </c>
@@ -19822,7 +19825,7 @@
       </c>
       <c r="L142" s="22"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A143" s="21">
         <v>2460</v>
       </c>
@@ -19847,7 +19850,7 @@
       </c>
       <c r="L143" s="22"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" s="21">
         <v>2462</v>
       </c>
@@ -19872,7 +19875,7 @@
       </c>
       <c r="L144" s="22"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" s="21">
         <v>2468</v>
       </c>
@@ -19897,7 +19900,7 @@
       </c>
       <c r="L145" s="22"/>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A146" s="21">
         <v>2471</v>
       </c>
@@ -19920,7 +19923,7 @@
       </c>
       <c r="L146" s="22"/>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A147" s="21">
         <v>2484</v>
       </c>
@@ -19945,7 +19948,7 @@
       </c>
       <c r="L147" s="22"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" s="21">
         <v>2550</v>
       </c>
@@ -19968,7 +19971,7 @@
       </c>
       <c r="L148" s="22"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" s="21">
         <v>2585</v>
       </c>
@@ -19983,91 +19986,91 @@
       <c r="K149" s="22"/>
       <c r="L149" s="22"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A150" s="22"/>
       <c r="B150" s="6"/>
       <c r="C150" s="6"/>
       <c r="D150" s="6"/>
       <c r="K150" s="6"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A151" s="6"/>
       <c r="B151" s="6"/>
       <c r="C151" s="6"/>
       <c r="D151" s="6"/>
       <c r="K151" s="6"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A152" s="6"/>
       <c r="B152" s="6"/>
       <c r="C152" s="6"/>
       <c r="D152" s="6"/>
       <c r="K152" s="6"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="6"/>
       <c r="B153" s="6"/>
       <c r="C153" s="6"/>
       <c r="D153" s="6"/>
       <c r="K153" s="6"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A154" s="6"/>
       <c r="B154" s="6"/>
       <c r="C154" s="6"/>
       <c r="D154" s="6"/>
       <c r="K154" s="6"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A155" s="6"/>
       <c r="B155" s="6"/>
       <c r="C155" s="6"/>
       <c r="D155" s="6"/>
       <c r="K155" s="6"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A156" s="6"/>
       <c r="B156" s="6"/>
       <c r="C156" s="6"/>
       <c r="D156" s="6"/>
       <c r="K156" s="6"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A157" s="6"/>
       <c r="B157" s="6"/>
       <c r="C157" s="6"/>
       <c r="D157" s="6"/>
       <c r="K157" s="6"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A158" s="6"/>
       <c r="B158" s="6"/>
       <c r="C158" s="6"/>
       <c r="D158" s="6"/>
       <c r="K158" s="6"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A159" s="6"/>
       <c r="B159" s="6"/>
       <c r="C159" s="6"/>
       <c r="D159" s="6"/>
       <c r="K159" s="6"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A160" s="6"/>
       <c r="B160" s="6"/>
       <c r="C160" s="6"/>
       <c r="D160" s="6"/>
       <c r="K160" s="6"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A161" s="6"/>
       <c r="B161" s="6"/>
       <c r="C161" s="6"/>
       <c r="D161" s="6"/>
       <c r="K161" s="6"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A162" s="6"/>
       <c r="B162" s="6"/>
       <c r="C162" s="6"/>
@@ -20075,98 +20078,98 @@
       <c r="K162" s="6"/>
       <c r="L162" s="6"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A163" s="6"/>
       <c r="B163" s="6"/>
       <c r="C163" s="6"/>
       <c r="D163" s="6"/>
       <c r="K163" s="6"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A164" s="6"/>
       <c r="B164" s="6"/>
       <c r="C164" s="6"/>
       <c r="D164" s="6"/>
       <c r="K164" s="6"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A165" s="6"/>
       <c r="B165" s="6"/>
       <c r="C165" s="6"/>
       <c r="D165" s="6"/>
       <c r="K165" s="6"/>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A166" s="6"/>
       <c r="B166" s="6"/>
       <c r="C166" s="6"/>
       <c r="D166" s="6"/>
       <c r="K166" s="6"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" s="6"/>
       <c r="B167" s="6"/>
       <c r="C167" s="6"/>
       <c r="D167" s="6"/>
       <c r="K167" s="6"/>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A168" s="6"/>
       <c r="B168" s="6"/>
       <c r="C168" s="6"/>
       <c r="D168" s="6"/>
       <c r="K168" s="6"/>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A169" s="6"/>
       <c r="B169" s="6"/>
       <c r="C169" s="6"/>
       <c r="D169" s="6"/>
       <c r="K169" s="6"/>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A170" s="6"/>
       <c r="B170" s="6"/>
       <c r="C170" s="6"/>
       <c r="D170" s="6"/>
       <c r="K170" s="6"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A171" s="6"/>
       <c r="B171" s="6"/>
       <c r="C171" s="6"/>
       <c r="D171" s="6"/>
       <c r="K171" s="6"/>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A172" s="6"/>
       <c r="B172" s="6"/>
       <c r="C172" s="6"/>
       <c r="D172" s="6"/>
       <c r="K172" s="6"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A173" s="6"/>
       <c r="B173" s="6"/>
       <c r="C173" s="6"/>
       <c r="D173" s="6"/>
       <c r="K173" s="6"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A174" s="6"/>
       <c r="B174" s="6"/>
       <c r="C174" s="6"/>
       <c r="D174" s="6"/>
       <c r="K174" s="6"/>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A175" s="6"/>
       <c r="B175" s="6"/>
       <c r="C175" s="6"/>
       <c r="D175" s="6"/>
       <c r="K175" s="6"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A176" s="6"/>
       <c r="B176" s="6"/>
       <c r="C176" s="6"/>
@@ -20593,7 +20596,7 @@
   <dimension ref="A1:U235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -22411,7 +22414,7 @@
       </c>
       <c r="L73" s="22"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="21">
         <v>1445</v>
       </c>
@@ -22436,7 +22439,7 @@
       </c>
       <c r="L74" s="22"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="21">
         <v>1455</v>
       </c>
@@ -22461,7 +22464,7 @@
       </c>
       <c r="L75" s="22"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="21">
         <v>1458</v>
       </c>
@@ -22484,7 +22487,7 @@
       </c>
       <c r="L76" s="22"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="21">
         <v>1495</v>
       </c>
@@ -22509,7 +22512,7 @@
       </c>
       <c r="L77" s="22"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="21">
         <v>1499</v>
       </c>
@@ -22534,7 +22537,7 @@
       </c>
       <c r="L78" s="22"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="21">
         <v>1535</v>
       </c>
@@ -22561,7 +22564,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="21">
         <v>1580</v>
       </c>
@@ -22586,7 +22589,7 @@
       </c>
       <c r="L80" s="22"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="21">
         <v>1605</v>
       </c>
@@ -22609,7 +22612,7 @@
       </c>
       <c r="L81" s="22"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="21">
         <v>1616</v>
       </c>
@@ -22634,7 +22637,7 @@
       </c>
       <c r="L82" s="22"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="21">
         <v>1670</v>
       </c>
@@ -22659,7 +22662,7 @@
       </c>
       <c r="L83" s="22"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="21">
         <v>1681</v>
       </c>
@@ -22684,7 +22687,7 @@
       </c>
       <c r="L84" s="22"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="21">
         <v>1745</v>
       </c>
@@ -22707,7 +22710,7 @@
       </c>
       <c r="L85" s="22"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="21">
         <v>1760</v>
       </c>
@@ -22732,7 +22735,7 @@
       </c>
       <c r="L86" s="22"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="21">
         <v>1771</v>
       </c>
@@ -22757,7 +22760,7 @@
       </c>
       <c r="L87" s="22"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="21">
         <v>1784</v>
       </c>
@@ -22780,7 +22783,7 @@
       </c>
       <c r="L88" s="22"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="21">
         <v>1786</v>
       </c>
@@ -22805,7 +22808,7 @@
       </c>
       <c r="L89" s="22"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="21">
         <v>1797</v>
       </c>
@@ -22828,7 +22831,7 @@
       </c>
       <c r="L90" s="22"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="21">
         <v>1804</v>
       </c>
@@ -22853,7 +22856,7 @@
       </c>
       <c r="L91" s="22"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="21">
         <v>1808</v>
       </c>
@@ -22876,7 +22879,7 @@
       </c>
       <c r="L92" s="22"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="21">
         <v>1812</v>
       </c>
@@ -22901,7 +22904,7 @@
       </c>
       <c r="L93" s="22"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="21">
         <v>1820</v>
       </c>
@@ -22924,7 +22927,7 @@
       </c>
       <c r="L94" s="22"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="21">
         <v>1826</v>
       </c>
@@ -22949,7 +22952,7 @@
       </c>
       <c r="L95" s="22"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="21">
         <v>1831</v>
       </c>
@@ -22974,7 +22977,7 @@
       </c>
       <c r="L96" s="22"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="21">
         <v>1903</v>
       </c>
@@ -22997,7 +23000,7 @@
       </c>
       <c r="L97" s="22"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="21">
         <v>1905</v>
       </c>
@@ -23022,7 +23025,7 @@
       </c>
       <c r="L98" s="22"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="21">
         <v>1907</v>
       </c>
@@ -23047,7 +23050,7 @@
       </c>
       <c r="L99" s="22"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="21">
         <v>1910</v>
       </c>
@@ -23072,7 +23075,7 @@
       </c>
       <c r="L100" s="22"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="21">
         <v>1915</v>
       </c>
@@ -23097,7 +23100,7 @@
       </c>
       <c r="L101" s="22"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="21">
         <v>1919</v>
       </c>
@@ -23122,7 +23125,7 @@
       </c>
       <c r="L102" s="22"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="21">
         <v>1925</v>
       </c>
@@ -23147,7 +23150,7 @@
       </c>
       <c r="L103" s="22"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="21">
         <v>1927</v>
       </c>
@@ -23172,7 +23175,7 @@
       </c>
       <c r="L104" s="22"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="21">
         <v>1968</v>
       </c>
@@ -23197,7 +23200,7 @@
       </c>
       <c r="L105" s="22"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="21">
         <v>1983</v>
       </c>
@@ -23224,7 +23227,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="21">
         <v>2010</v>
       </c>
@@ -23251,7 +23254,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="21">
         <v>2040</v>
       </c>
@@ -23278,7 +23281,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="21">
         <v>2111</v>
       </c>
@@ -23303,7 +23306,7 @@
       </c>
       <c r="L109" s="22"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" s="21">
         <v>2119</v>
       </c>
@@ -23328,7 +23331,7 @@
       </c>
       <c r="L110" s="22"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="21">
         <v>2232</v>
       </c>
@@ -23353,7 +23356,7 @@
       </c>
       <c r="L111" s="22"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="21">
         <v>2240</v>
       </c>
@@ -23378,7 +23381,7 @@
       </c>
       <c r="L112" s="22"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="21">
         <v>2275</v>
       </c>
@@ -23403,7 +23406,7 @@
       </c>
       <c r="L113" s="22"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="21">
         <v>2279</v>
       </c>
@@ -23428,7 +23431,7 @@
       </c>
       <c r="L114" s="22"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="21">
         <v>2303</v>
       </c>
@@ -23453,7 +23456,7 @@
       </c>
       <c r="L115" s="22"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="21">
         <v>2312</v>
       </c>
@@ -23478,7 +23481,7 @@
       </c>
       <c r="L116" s="22"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="21">
         <v>2360</v>
       </c>
@@ -23503,7 +23506,7 @@
       </c>
       <c r="L117" s="22"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="21">
         <v>2364</v>
       </c>
@@ -23528,7 +23531,7 @@
       </c>
       <c r="L118" s="22"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="21">
         <v>2482</v>
       </c>
@@ -23549,7 +23552,7 @@
       <c r="K119" s="22"/>
       <c r="L119" s="22"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="21">
         <v>2506</v>
       </c>
@@ -23574,7 +23577,7 @@
       </c>
       <c r="L120" s="22"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="21">
         <v>2511</v>
       </c>
@@ -23599,7 +23602,7 @@
       </c>
       <c r="L121" s="22"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="21">
         <v>2540</v>
       </c>
@@ -23624,7 +23627,7 @@
       </c>
       <c r="L122" s="22"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="21">
         <v>2580</v>
       </c>
@@ -23649,7 +23652,7 @@
       </c>
       <c r="L123" s="22"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="21">
         <v>2588</v>
       </c>
@@ -23674,7 +23677,7 @@
       </c>
       <c r="L124" s="22"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="21">
         <v>2609</v>
       </c>
@@ -23699,7 +23702,7 @@
       </c>
       <c r="L125" s="22"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" s="21">
         <v>2632</v>
       </c>
@@ -23724,7 +23727,7 @@
       </c>
       <c r="L126" s="22"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A127" s="21">
         <v>2641</v>
       </c>
@@ -23749,7 +23752,7 @@
       </c>
       <c r="L127" s="22"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A128" s="21">
         <v>2700</v>
       </c>
@@ -23764,7 +23767,7 @@
       <c r="K128" s="22"/>
       <c r="L128" s="22"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A129" s="22" t="s">
         <v>122</v>
       </c>
@@ -23773,119 +23776,119 @@
       <c r="D129" s="6"/>
       <c r="K129" s="6"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" s="6"/>
       <c r="B130" s="6"/>
       <c r="C130" s="6"/>
       <c r="D130" s="6"/>
       <c r="K130" s="6"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="6"/>
       <c r="B131" s="6"/>
       <c r="C131" s="6"/>
       <c r="D131" s="6"/>
       <c r="K131" s="6"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="6"/>
       <c r="B132" s="6"/>
       <c r="C132" s="6"/>
       <c r="D132" s="6"/>
       <c r="K132" s="6"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="6"/>
       <c r="B133" s="6"/>
       <c r="C133" s="6"/>
       <c r="D133" s="6"/>
       <c r="K133" s="6"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="6"/>
       <c r="B134" s="6"/>
       <c r="C134" s="6"/>
       <c r="D134" s="6"/>
       <c r="K134" s="6"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A135" s="6"/>
       <c r="B135" s="6"/>
       <c r="C135" s="6"/>
       <c r="D135" s="6"/>
       <c r="K135" s="6"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A136" s="6"/>
       <c r="B136" s="6"/>
       <c r="C136" s="6"/>
       <c r="D136" s="6"/>
       <c r="K136" s="6"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A137" s="6"/>
       <c r="B137" s="6"/>
       <c r="C137" s="6"/>
       <c r="D137" s="6"/>
       <c r="K137" s="6"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A138" s="6"/>
       <c r="B138" s="6"/>
       <c r="C138" s="6"/>
       <c r="D138" s="6"/>
       <c r="K138" s="6"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A139" s="6"/>
       <c r="B139" s="6"/>
       <c r="C139" s="6"/>
       <c r="D139" s="6"/>
       <c r="K139" s="6"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" s="6"/>
       <c r="B140" s="6"/>
       <c r="C140" s="6"/>
       <c r="D140" s="6"/>
       <c r="K140" s="6"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A141" s="6"/>
       <c r="B141" s="6"/>
       <c r="C141" s="6"/>
       <c r="D141" s="6"/>
       <c r="K141" s="6"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="6"/>
       <c r="B142" s="6"/>
       <c r="C142" s="6"/>
       <c r="D142" s="6"/>
       <c r="K142" s="6"/>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A143" s="6"/>
       <c r="B143" s="6"/>
       <c r="C143" s="6"/>
       <c r="D143" s="6"/>
       <c r="K143" s="6"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" s="6"/>
       <c r="B144" s="6"/>
       <c r="C144" s="6"/>
       <c r="D144" s="6"/>
       <c r="K144" s="6"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" s="6"/>
       <c r="B145" s="6"/>
       <c r="C145" s="6"/>
       <c r="D145" s="6"/>
       <c r="K145" s="6"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A146" s="6"/>
       <c r="B146" s="6"/>
       <c r="C146" s="6"/>
@@ -23893,119 +23896,119 @@
       <c r="F146" s="12"/>
       <c r="K146" s="6"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A147" s="6"/>
       <c r="B147" s="6"/>
       <c r="C147" s="6"/>
       <c r="D147" s="6"/>
       <c r="K147" s="6"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" s="6"/>
       <c r="B148" s="6"/>
       <c r="C148" s="6"/>
       <c r="D148" s="6"/>
       <c r="K148" s="6"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" s="6"/>
       <c r="B149" s="6"/>
       <c r="C149" s="6"/>
       <c r="D149" s="6"/>
       <c r="K149" s="6"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A150" s="6"/>
       <c r="B150" s="6"/>
       <c r="C150" s="6"/>
       <c r="D150" s="6"/>
       <c r="K150" s="6"/>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A151" s="6"/>
       <c r="B151" s="6"/>
       <c r="C151" s="6"/>
       <c r="D151" s="6"/>
       <c r="K151" s="6"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A152" s="6"/>
       <c r="B152" s="6"/>
       <c r="C152" s="6"/>
       <c r="D152" s="6"/>
       <c r="K152" s="6"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="6"/>
       <c r="B153" s="6"/>
       <c r="C153" s="6"/>
       <c r="D153" s="6"/>
       <c r="K153" s="6"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A154" s="6"/>
       <c r="B154" s="6"/>
       <c r="C154" s="6"/>
       <c r="D154" s="6"/>
       <c r="K154" s="6"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A155" s="6"/>
       <c r="B155" s="6"/>
       <c r="C155" s="6"/>
       <c r="D155" s="6"/>
       <c r="K155" s="6"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A156" s="6"/>
       <c r="B156" s="6"/>
       <c r="C156" s="6"/>
       <c r="D156" s="6"/>
       <c r="K156" s="6"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A157" s="6"/>
       <c r="B157" s="6"/>
       <c r="C157" s="6"/>
       <c r="D157" s="6"/>
       <c r="K157" s="6"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A158" s="6"/>
       <c r="B158" s="6"/>
       <c r="C158" s="6"/>
       <c r="D158" s="6"/>
       <c r="K158" s="6"/>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A159" s="6"/>
       <c r="B159" s="6"/>
       <c r="C159" s="6"/>
       <c r="D159" s="6"/>
       <c r="K159" s="6"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A160" s="6"/>
       <c r="B160" s="6"/>
       <c r="C160" s="6"/>
       <c r="D160" s="6"/>
       <c r="K160" s="6"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A161" s="6"/>
       <c r="B161" s="6"/>
       <c r="C161" s="6"/>
       <c r="D161" s="6"/>
       <c r="K161" s="6"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A162" s="6"/>
       <c r="B162" s="6"/>
       <c r="C162" s="6"/>
       <c r="D162" s="6"/>
       <c r="K162" s="6"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A163" s="6"/>
       <c r="B163" s="6"/>
       <c r="C163" s="6"/>
@@ -24013,392 +24016,392 @@
       <c r="K163" s="6"/>
       <c r="L163" s="6"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A164" s="6"/>
       <c r="B164" s="6"/>
       <c r="C164" s="6"/>
       <c r="D164" s="6"/>
       <c r="K164" s="6"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A165" s="6"/>
       <c r="B165" s="6"/>
       <c r="C165" s="6"/>
       <c r="D165" s="6"/>
       <c r="K165" s="6"/>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A166" s="6"/>
       <c r="B166" s="6"/>
       <c r="C166" s="6"/>
       <c r="D166" s="6"/>
       <c r="K166" s="6"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" s="6"/>
       <c r="B167" s="6"/>
       <c r="C167" s="6"/>
       <c r="D167" s="6"/>
       <c r="K167" s="6"/>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A168" s="6"/>
       <c r="B168" s="6"/>
       <c r="C168" s="6"/>
       <c r="D168" s="6"/>
       <c r="K168" s="6"/>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A169" s="6"/>
       <c r="B169" s="6"/>
       <c r="C169" s="6"/>
       <c r="D169" s="6"/>
       <c r="K169" s="6"/>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A170" s="6"/>
       <c r="B170" s="6"/>
       <c r="C170" s="6"/>
       <c r="D170" s="6"/>
       <c r="K170" s="6"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A171" s="6"/>
       <c r="B171" s="6"/>
       <c r="C171" s="6"/>
       <c r="D171" s="6"/>
       <c r="K171" s="6"/>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A172" s="6"/>
       <c r="B172" s="6"/>
       <c r="C172" s="6"/>
       <c r="D172" s="6"/>
       <c r="K172" s="6"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A173" s="6"/>
       <c r="B173" s="6"/>
       <c r="C173" s="6"/>
       <c r="D173" s="6"/>
       <c r="K173" s="6"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A174" s="6"/>
       <c r="B174" s="6"/>
       <c r="C174" s="6"/>
       <c r="D174" s="6"/>
       <c r="K174" s="6"/>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A175" s="6"/>
       <c r="B175" s="6"/>
       <c r="C175" s="6"/>
       <c r="D175" s="6"/>
       <c r="K175" s="6"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A176" s="6"/>
       <c r="B176" s="6"/>
       <c r="C176" s="6"/>
       <c r="D176" s="6"/>
       <c r="K176" s="6"/>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A177" s="6"/>
       <c r="B177" s="6"/>
       <c r="C177" s="6"/>
       <c r="D177" s="6"/>
       <c r="K177" s="6"/>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A178" s="6"/>
       <c r="B178" s="6"/>
       <c r="C178" s="6"/>
       <c r="D178" s="6"/>
       <c r="K178" s="6"/>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A179" s="6"/>
       <c r="B179" s="6"/>
       <c r="C179" s="6"/>
       <c r="D179" s="6"/>
       <c r="K179" s="6"/>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A180" s="6"/>
       <c r="B180" s="6"/>
       <c r="C180" s="6"/>
       <c r="D180" s="6"/>
       <c r="K180" s="6"/>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A181" s="6"/>
       <c r="B181" s="6"/>
       <c r="C181" s="6"/>
       <c r="D181" s="6"/>
       <c r="K181" s="6"/>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A182" s="6"/>
       <c r="B182" s="6"/>
       <c r="C182" s="6"/>
       <c r="D182" s="6"/>
       <c r="K182" s="6"/>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A183" s="6"/>
       <c r="B183" s="6"/>
       <c r="C183" s="6"/>
       <c r="D183" s="6"/>
       <c r="K183" s="6"/>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A184" s="6"/>
       <c r="B184" s="6"/>
       <c r="C184" s="6"/>
       <c r="D184" s="6"/>
       <c r="K184" s="6"/>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A185" s="6"/>
       <c r="B185" s="6"/>
       <c r="C185" s="6"/>
       <c r="D185" s="6"/>
       <c r="K185" s="6"/>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A186" s="6"/>
       <c r="B186" s="6"/>
       <c r="C186" s="6"/>
       <c r="D186" s="6"/>
       <c r="K186" s="6"/>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A187" s="6"/>
       <c r="B187" s="6"/>
       <c r="C187" s="6"/>
       <c r="D187" s="6"/>
       <c r="K187" s="6"/>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A188" s="6"/>
       <c r="B188" s="6"/>
       <c r="C188" s="6"/>
       <c r="D188" s="6"/>
       <c r="K188" s="6"/>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A189" s="6"/>
       <c r="B189" s="6"/>
       <c r="C189" s="6"/>
       <c r="D189" s="6"/>
       <c r="K189" s="6"/>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A190" s="6"/>
       <c r="B190" s="6"/>
       <c r="C190" s="6"/>
       <c r="D190" s="6"/>
       <c r="K190" s="6"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A191" s="6"/>
       <c r="B191" s="6"/>
       <c r="C191" s="6"/>
       <c r="D191" s="6"/>
       <c r="K191" s="6"/>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A192" s="6"/>
       <c r="B192" s="6"/>
       <c r="C192" s="6"/>
       <c r="D192" s="6"/>
       <c r="K192" s="6"/>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A193" s="6"/>
       <c r="B193" s="6"/>
       <c r="C193" s="6"/>
       <c r="D193" s="6"/>
       <c r="K193" s="6"/>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A194" s="6"/>
       <c r="B194" s="6"/>
       <c r="C194" s="6"/>
       <c r="D194" s="6"/>
       <c r="K194" s="6"/>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A195" s="6"/>
       <c r="B195" s="6"/>
       <c r="C195" s="6"/>
       <c r="D195" s="6"/>
       <c r="K195" s="6"/>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A196" s="6"/>
       <c r="B196" s="6"/>
       <c r="C196" s="6"/>
       <c r="D196" s="6"/>
       <c r="K196" s="6"/>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A197" s="6"/>
       <c r="B197" s="6"/>
       <c r="C197" s="6"/>
       <c r="D197" s="6"/>
       <c r="K197" s="6"/>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A198" s="6"/>
       <c r="B198" s="6"/>
       <c r="C198" s="6"/>
       <c r="D198" s="6"/>
       <c r="K198" s="6"/>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A199" s="6"/>
       <c r="B199" s="6"/>
       <c r="C199" s="6"/>
       <c r="D199" s="6"/>
       <c r="K199" s="6"/>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A200" s="6"/>
       <c r="B200" s="6"/>
       <c r="C200" s="6"/>
       <c r="D200" s="6"/>
       <c r="K200" s="6"/>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A201" s="6"/>
       <c r="B201" s="6"/>
       <c r="C201" s="6"/>
       <c r="D201" s="6"/>
       <c r="K201" s="6"/>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A202" s="6"/>
       <c r="B202" s="6"/>
       <c r="C202" s="6"/>
       <c r="D202" s="6"/>
       <c r="K202" s="6"/>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A203" s="6"/>
       <c r="B203" s="6"/>
       <c r="C203" s="6"/>
       <c r="D203" s="6"/>
       <c r="K203" s="6"/>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A204" s="6"/>
       <c r="B204" s="6"/>
       <c r="C204" s="6"/>
       <c r="D204" s="6"/>
       <c r="K204" s="6"/>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A205" s="6"/>
       <c r="B205" s="6"/>
       <c r="C205" s="6"/>
       <c r="D205" s="6"/>
       <c r="K205" s="6"/>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A206" s="6"/>
       <c r="B206" s="6"/>
       <c r="C206" s="6"/>
       <c r="D206" s="6"/>
       <c r="K206" s="6"/>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A207" s="6"/>
       <c r="B207" s="6"/>
       <c r="C207" s="6"/>
       <c r="D207" s="6"/>
       <c r="K207" s="6"/>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A208" s="6"/>
       <c r="B208" s="6"/>
       <c r="C208" s="6"/>
       <c r="D208" s="6"/>
       <c r="K208" s="6"/>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A209" s="6"/>
       <c r="B209" s="6"/>
       <c r="C209" s="6"/>
       <c r="D209" s="6"/>
       <c r="K209" s="6"/>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A210" s="6"/>
       <c r="B210" s="6"/>
       <c r="C210" s="6"/>
       <c r="D210" s="6"/>
       <c r="K210" s="6"/>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A211" s="6"/>
       <c r="B211" s="6"/>
       <c r="C211" s="6"/>
       <c r="D211" s="6"/>
       <c r="K211" s="6"/>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A212" s="6"/>
       <c r="B212" s="6"/>
       <c r="C212" s="6"/>
       <c r="D212" s="6"/>
       <c r="K212" s="6"/>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A213" s="6"/>
       <c r="B213" s="6"/>
       <c r="C213" s="6"/>
       <c r="D213" s="6"/>
       <c r="K213" s="6"/>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A214" s="6"/>
       <c r="B214" s="6"/>
       <c r="C214" s="6"/>
       <c r="D214" s="6"/>
       <c r="K214" s="6"/>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A215" s="6"/>
       <c r="B215" s="6"/>
       <c r="C215" s="6"/>
       <c r="D215" s="6"/>
       <c r="K215" s="6"/>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A216" s="6"/>
       <c r="B216" s="6"/>
       <c r="C216" s="6"/>
       <c r="D216" s="6"/>
       <c r="K216" s="6"/>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A217" s="6"/>
       <c r="B217" s="6"/>
       <c r="C217" s="6"/>
       <c r="D217" s="6"/>
       <c r="K217" s="6"/>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A218" s="6"/>
       <c r="B218" s="6"/>
       <c r="C218" s="6"/>
       <c r="D218" s="6"/>
       <c r="K218" s="6"/>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A219" s="6"/>
       <c r="B219" s="6"/>
       <c r="C219" s="6"/>
@@ -24406,113 +24409,114 @@
       <c r="K219" s="6"/>
       <c r="L219" s="6"/>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A220" s="6"/>
       <c r="B220" s="6"/>
       <c r="C220" s="6"/>
       <c r="D220" s="6"/>
       <c r="K220" s="6"/>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A221" s="6"/>
       <c r="B221" s="6"/>
       <c r="C221" s="6"/>
       <c r="D221" s="6"/>
       <c r="K221" s="6"/>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A222" s="6"/>
       <c r="B222" s="6"/>
       <c r="C222" s="6"/>
       <c r="D222" s="6"/>
       <c r="K222" s="6"/>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A223" s="6"/>
       <c r="B223" s="6"/>
       <c r="C223" s="6"/>
       <c r="D223" s="6"/>
       <c r="K223" s="6"/>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A224" s="6"/>
       <c r="B224" s="6"/>
       <c r="C224" s="6"/>
       <c r="D224" s="6"/>
       <c r="K224" s="6"/>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A225" s="6"/>
       <c r="B225" s="6"/>
       <c r="C225" s="6"/>
       <c r="D225" s="6"/>
       <c r="K225" s="6"/>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A226" s="6"/>
       <c r="B226" s="6"/>
       <c r="C226" s="6"/>
       <c r="D226" s="6"/>
       <c r="K226" s="6"/>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A227" s="6"/>
       <c r="B227" s="6"/>
       <c r="C227" s="6"/>
       <c r="D227" s="6"/>
       <c r="K227" s="6"/>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A228" s="6"/>
       <c r="B228" s="6"/>
       <c r="C228" s="6"/>
       <c r="D228" s="6"/>
       <c r="K228" s="6"/>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A229" s="6"/>
       <c r="B229" s="6"/>
       <c r="C229" s="6"/>
       <c r="D229" s="6"/>
       <c r="K229" s="6"/>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A230" s="6"/>
       <c r="B230" s="6"/>
       <c r="C230" s="6"/>
       <c r="D230" s="6"/>
       <c r="K230" s="6"/>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A231" s="6"/>
       <c r="B231" s="6"/>
       <c r="C231" s="6"/>
       <c r="D231" s="6"/>
       <c r="K231" s="6"/>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A232" s="6"/>
       <c r="B232" s="6"/>
       <c r="C232" s="6"/>
       <c r="D232" s="6"/>
       <c r="K232" s="6"/>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A233" s="6"/>
       <c r="B233" s="6"/>
       <c r="C233" s="6"/>
       <c r="D233" s="6"/>
       <c r="K233" s="6"/>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A234" s="6"/>
       <c r="C234" s="6"/>
       <c r="K234" s="6"/>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A235" s="6"/>
     </row>
   </sheetData>
+  <autoFilter ref="A4:U129" xr:uid="{00000000-0001-0000-0600-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="K70:L70"/>
   </mergeCells>

</xml_diff>